<commit_message>
MiniGraficos - Finalização módulo 07
</commit_message>
<xml_diff>
--- a/módulo 07/aula-minigraficos.xlsx
+++ b/módulo 07/aula-minigraficos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelio\Google Drive\Cursos online\Curso_Excel\07 Graficos e Minigráficos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\módulo 07\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" tabRatio="741"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="741"/>
   </bookViews>
   <sheets>
     <sheet name="Desempenho da Frota" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="36">
   <si>
     <t>VEÍCULO</t>
   </si>
@@ -97,6 +97,42 @@
   </si>
   <si>
     <t>META MENSAL:</t>
+  </si>
+  <si>
+    <t>Inserir minigráfico: aba inserir/minigráficos/seleciona o intervalo de dados/</t>
+  </si>
+  <si>
+    <t>enter/seleciona a célula onde o gráfico deverá aparecer</t>
+  </si>
+  <si>
+    <t>Saber a quem o mingráfico pertence: clica em cima do gráfico/aba design/editar dados</t>
+  </si>
+  <si>
+    <t>editar dados do minigráfico unico. Isso levará até o intervalo de dados a qual o gráfico pertence</t>
+  </si>
+  <si>
+    <t>Ponto alto/baixo: clica no gráfico/aba design/ponto alto/baixo</t>
+  </si>
+  <si>
+    <t>Os gráficos estão agrupados por padrão</t>
+  </si>
+  <si>
+    <t>Formatar: clica no gráfico/design/cor do minigráfico ou cor do marcador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para facilitar a comparação dos dados no minigráfico marque a max e min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">para: igual para todos os gráficos. Ex: clica no gráfico/design/eixo/opções </t>
+  </si>
+  <si>
+    <t>de valores max/min de eixo vertical/marque a opção igual para todos</t>
+  </si>
+  <si>
+    <t>Fazer os gráficos aparecerem mesmo com as células ocultas: seleciona o gráfico</t>
+  </si>
+  <si>
+    <t>aba design/editar dados/celulas ocultas e vazias/marca a opção: mostrar dados em linhas e colunas ocultas</t>
   </si>
 </sst>
 </file>
@@ -277,7 +313,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B530947-99D5-4D97-B33F-F3233C606F56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9B530947-99D5-4D97-B33F-F3233C606F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -356,7 +392,7 @@
         <xdr:cNvPr id="4" name="CaixaDeTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B530947-99D5-4D97-B33F-F3233C606F56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9B530947-99D5-4D97-B33F-F3233C606F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -468,7 +504,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B530947-99D5-4D97-B33F-F3233C606F56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9B530947-99D5-4D97-B33F-F3233C606F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -547,7 +583,7 @@
         <xdr:cNvPr id="4" name="CaixaDeTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B530947-99D5-4D97-B33F-F3233C606F56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9B530947-99D5-4D97-B33F-F3233C606F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -936,16 +972,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S22"/>
+  <dimension ref="B1:S29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="5" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="19" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" hidden="1"/>
+    <col min="8" max="16384" width="12.7109375" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -963,7 +1003,7 @@
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1056,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
@@ -1063,7 +1103,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
@@ -1110,7 +1150,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="8" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
@@ -1157,7 +1197,7 @@
         <v>4.3899999999999997</v>
       </c>
     </row>
-    <row r="9" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>4</v>
       </c>
@@ -1288,6 +1328,9 @@
       </c>
     </row>
     <row r="13" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
       <c r="G13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1329,6 +1372,9 @@
       </c>
     </row>
     <row r="14" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
       <c r="E14" s="13"/>
       <c r="G14" s="3" t="s">
         <v>5</v>
@@ -1371,6 +1417,9 @@
       </c>
     </row>
     <row r="15" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
       <c r="G15" s="6" t="s">
         <v>4</v>
       </c>
@@ -1412,8 +1461,15 @@
       </c>
     </row>
     <row r="16" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="7:19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="7:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
       <c r="G18" s="4" t="s">
         <v>21</v>
       </c>
@@ -1454,7 +1510,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="7:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G19" s="5" t="s">
         <v>7</v>
       </c>
@@ -1507,7 +1563,10 @@
         <v>15781</v>
       </c>
     </row>
-    <row r="20" spans="7:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
       <c r="G20" s="3" t="s">
         <v>6</v>
       </c>
@@ -1560,7 +1619,7 @@
         <v>-1971</v>
       </c>
     </row>
-    <row r="21" spans="7:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G21" s="3" t="s">
         <v>5</v>
       </c>
@@ -1613,7 +1672,10 @@
         <v>8960</v>
       </c>
     </row>
-    <row r="22" spans="7:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
       <c r="G22" s="6" t="s">
         <v>4</v>
       </c>
@@ -1664,12 +1726,127 @@
       <c r="S22" s="9">
         <f t="shared" si="3"/>
         <v>-3864</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" high="1" low="1" displayHidden="1" minAxisType="group" maxAxisType="group">
+          <x14:colorSeries theme="9" tint="-0.249977111117893"/>
+          <x14:colorNegative theme="1" tint="0.249977111117893"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="1" tint="0.249977111117893"/>
+          <x14:colorFirst theme="1" tint="0.249977111117893"/>
+          <x14:colorLast theme="1" tint="0.249977111117893"/>
+          <x14:colorHigh theme="4" tint="-0.249977111117893"/>
+          <x14:colorLow rgb="FFC00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Desempenho da Frota'!H6:S6</xm:f>
+              <xm:sqref>C6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Desempenho da Frota'!H7:S7</xm:f>
+              <xm:sqref>C7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Desempenho da Frota'!H8:S8</xm:f>
+              <xm:sqref>C8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Desempenho da Frota'!H9:S9</xm:f>
+              <xm:sqref>C9</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="stacked" displayEmptyCellsAs="gap" negative="1" displayXAxis="1" displayHidden="1" minAxisType="group" maxAxisType="group">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh theme="9" tint="-0.249977111117893"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Desempenho da Frota'!H19:S19</xm:f>
+              <xm:sqref>E6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Desempenho da Frota'!H20:S20</xm:f>
+              <xm:sqref>E7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Desempenho da Frota'!H21:S21</xm:f>
+              <xm:sqref>E8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Desempenho da Frota'!H22:S22</xm:f>
+              <xm:sqref>E9</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" high="1" low="1" displayHidden="1" minAxisType="group" maxAxisType="group">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh theme="9" tint="-0.249977111117893"/>
+          <x14:colorLow rgb="FFC00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Desempenho da Frota'!H12:S12</xm:f>
+              <xm:sqref>D6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Desempenho da Frota'!H13:S13</xm:f>
+              <xm:sqref>D7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Desempenho da Frota'!H14:S14</xm:f>
+              <xm:sqref>D8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Desempenho da Frota'!H15:S15</xm:f>
+              <xm:sqref>D9</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2403,31 +2580,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" high="1" low="1" displayHidden="1" minAxisType="group" maxAxisType="group">
+        <x14:sparklineGroup manualMax="5" manualMin="3" lineWeight="1.5" displayEmptyCellsAs="gap" high="1" low="1" displayHidden="1" minAxisType="custom" maxAxisType="custom">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
           <x14:colorMarkers rgb="FFD00000"/>
           <x14:colorFirst rgb="FFD00000"/>
           <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh theme="9" tint="-0.249977111117893"/>
-          <x14:colorLow rgb="FFFF0000"/>
+          <x14:colorHigh rgb="FF00B050"/>
+          <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Desempenho da Frota - Final'!H12:S12</xm:f>
-              <xm:sqref>D6</xm:sqref>
+              <xm:f>'Desempenho da Frota - Final'!H6:S6</xm:f>
+              <xm:sqref>C6</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>'Desempenho da Frota - Final'!H13:S13</xm:f>
-              <xm:sqref>D7</xm:sqref>
+              <xm:f>'Desempenho da Frota - Final'!H7:S7</xm:f>
+              <xm:sqref>C7</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>'Desempenho da Frota - Final'!H14:S14</xm:f>
-              <xm:sqref>D8</xm:sqref>
+              <xm:f>'Desempenho da Frota - Final'!H8:S8</xm:f>
+              <xm:sqref>C8</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>'Desempenho da Frota - Final'!H15:S15</xm:f>
-              <xm:sqref>D9</xm:sqref>
+              <xm:f>'Desempenho da Frota - Final'!H9:S9</xm:f>
+              <xm:sqref>C9</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -2459,31 +2636,31 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup manualMax="5" manualMin="3" lineWeight="1.5" displayEmptyCellsAs="gap" high="1" low="1" displayHidden="1" minAxisType="custom" maxAxisType="custom">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" high="1" low="1" displayHidden="1" minAxisType="group" maxAxisType="group">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
           <x14:colorMarkers rgb="FFD00000"/>
           <x14:colorFirst rgb="FFD00000"/>
           <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FF00B050"/>
-          <x14:colorLow rgb="FFD00000"/>
+          <x14:colorHigh theme="9" tint="-0.249977111117893"/>
+          <x14:colorLow rgb="FFFF0000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Desempenho da Frota - Final'!H6:S6</xm:f>
-              <xm:sqref>C6</xm:sqref>
+              <xm:f>'Desempenho da Frota - Final'!H12:S12</xm:f>
+              <xm:sqref>D6</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>'Desempenho da Frota - Final'!H7:S7</xm:f>
-              <xm:sqref>C7</xm:sqref>
+              <xm:f>'Desempenho da Frota - Final'!H13:S13</xm:f>
+              <xm:sqref>D7</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>'Desempenho da Frota - Final'!H8:S8</xm:f>
-              <xm:sqref>C8</xm:sqref>
+              <xm:f>'Desempenho da Frota - Final'!H14:S14</xm:f>
+              <xm:sqref>D8</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>'Desempenho da Frota - Final'!H9:S9</xm:f>
-              <xm:sqref>C9</xm:sqref>
+              <xm:f>'Desempenho da Frota - Final'!H15:S15</xm:f>
+              <xm:sqref>D9</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>